<commit_message>
add reports alluser, someevents, userregisteronevent; format date 2020-12-15
</commit_message>
<xml_diff>
--- a/registr.xlsx
+++ b/registr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>Номер_события</t>
   </si>
@@ -130,7 +130,37 @@
     <t>08.02.2020</t>
   </si>
   <si>
-    <t>2019-06-20 00:00:00</t>
+    <t>Студенческая олимпиада</t>
+  </si>
+  <si>
+    <t>Лингвистика</t>
+  </si>
+  <si>
+    <t>20.12.2020</t>
+  </si>
+  <si>
+    <t>Кудлай</t>
+  </si>
+  <si>
+    <t>Полина</t>
+  </si>
+  <si>
+    <t>Александровна</t>
+  </si>
+  <si>
+    <t>Иноватика</t>
+  </si>
+  <si>
+    <t>pol@ina.com</t>
+  </si>
+  <si>
+    <t>789654</t>
+  </si>
+  <si>
+    <t>15.11.1999</t>
+  </si>
+  <si>
+    <t>2019-07-24 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -462,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,8 +739,128 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
report about all registration, recovery password
</commit_message>
<xml_diff>
--- a/registr.xlsx
+++ b/registr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Номер_события</t>
   </si>
@@ -28,6 +28,15 @@
     <t>Дата _проведения</t>
   </si>
   <si>
+    <t>Время начала</t>
+  </si>
+  <si>
+    <t>Продолжительность</t>
+  </si>
+  <si>
+    <t>Адрес проведения</t>
+  </si>
+  <si>
     <t>Номер_волонтера</t>
   </si>
   <si>
@@ -43,7 +52,7 @@
     <t>Факультет</t>
   </si>
   <si>
-    <t>email</t>
+    <t>e-mail</t>
   </si>
   <si>
     <t>Телефон</t>
@@ -52,16 +61,28 @@
     <t>Дата_рождения</t>
   </si>
   <si>
+    <t>Пол</t>
+  </si>
+  <si>
+    <t>Курс</t>
+  </si>
+  <si>
     <t>Отметка_о_посещении</t>
   </si>
   <si>
+    <t>Роль выбраная при регистрации</t>
+  </si>
+  <si>
+    <t>Аудитория</t>
+  </si>
+  <si>
     <t>Высшая проба</t>
   </si>
   <si>
     <t>Математика</t>
   </si>
   <si>
-    <t>02.02.2020</t>
+    <t>2020-02-02</t>
   </si>
   <si>
     <t>Мрак</t>
@@ -124,43 +145,7 @@
     <t>11.11.2011</t>
   </si>
   <si>
-    <t>Филология</t>
-  </si>
-  <si>
-    <t>08.02.2020</t>
-  </si>
-  <si>
-    <t>Студенческая олимпиада</t>
-  </si>
-  <si>
-    <t>Лингвистика</t>
-  </si>
-  <si>
-    <t>20.12.2020</t>
-  </si>
-  <si>
-    <t>Кудлай</t>
-  </si>
-  <si>
-    <t>Полина</t>
-  </si>
-  <si>
-    <t>Александровна</t>
-  </si>
-  <si>
-    <t>Иноватика</t>
-  </si>
-  <si>
-    <t>pol@ina.com</t>
-  </si>
-  <si>
-    <t>789654</t>
-  </si>
-  <si>
-    <t>15.11.1999</t>
-  </si>
-  <si>
-    <t>2019-07-24 00:00:00</t>
+    <t>2019-07-25 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -492,13 +477,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,329 +523,151 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
+        <v>22</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
+      <c r="I3" t="s">
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regform on idex page, correct mistakes, sort news by date, limit on news
</commit_message>
<xml_diff>
--- a/registr.xlsx
+++ b/registr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
   <si>
     <t>Номер_события</t>
   </si>
@@ -76,6 +76,42 @@
     <t>Аудитория</t>
   </si>
   <si>
+    <t>Высшая проба</t>
+  </si>
+  <si>
+    <t>Коммандная олимпиада по программированию</t>
+  </si>
+  <si>
+    <t>2020-11-27</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>Мясницкая, 11</t>
+  </si>
+  <si>
+    <t>Суханов</t>
+  </si>
+  <si>
+    <t>Игорь</t>
+  </si>
+  <si>
+    <t>Константинович</t>
+  </si>
+  <si>
+    <t>you@me.they</t>
+  </si>
+  <si>
+    <t>456542145</t>
+  </si>
+  <si>
+    <t>21.11.2001</t>
+  </si>
+  <si>
+    <t>штаб</t>
+  </si>
+  <si>
     <t>Студенческая олимпиада</t>
   </si>
   <si>
@@ -88,27 +124,6 @@
     <t>10:00</t>
   </si>
   <si>
-    <t>Суханов</t>
-  </si>
-  <si>
-    <t>Игорь</t>
-  </si>
-  <si>
-    <t>Константинович</t>
-  </si>
-  <si>
-    <t>you@me.they</t>
-  </si>
-  <si>
-    <t>456542145</t>
-  </si>
-  <si>
-    <t>21.11.2001</t>
-  </si>
-  <si>
-    <t>штаб</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -139,9 +154,6 @@
     <t>555</t>
   </si>
   <si>
-    <t>Высшая проба</t>
-  </si>
-  <si>
     <t>Филология</t>
   </si>
   <si>
@@ -175,7 +187,7 @@
     <t>2020-02-02</t>
   </si>
   <si>
-    <t>2019-08-03 00:00:00</t>
+    <t>2019-09-07 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -577,7 +589,7 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -592,36 +604,36 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>280</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -630,93 +642,102 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>120</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="N4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="O4" t="s">
         <v>43</v>
       </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
+      <c r="T4" t="s">
         <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -724,81 +745,81 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="L5" t="s">
+        <v>51</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="R5">
         <v>0</v>
-      </c>
-      <c r="S5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
         <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -806,42 +827,45 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+      <c r="M7" t="s">
         <v>52</v>
       </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix error and view for reserve
</commit_message>
<xml_diff>
--- a/registr.xlsx
+++ b/registr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="205">
   <si>
     <t>Номер_события</t>
   </si>
@@ -76,6 +76,114 @@
     <t>Аудитория</t>
   </si>
   <si>
+    <t>Тест</t>
+  </si>
+  <si>
+    <t>Завершение отмены регистрации</t>
+  </si>
+  <si>
+    <t>2020-08-06</t>
+  </si>
+  <si>
+    <t>12:10</t>
+  </si>
+  <si>
+    <t>Онлайн</t>
+  </si>
+  <si>
+    <t>Петров</t>
+  </si>
+  <si>
+    <t>Петр</t>
+  </si>
+  <si>
+    <t>Петрович</t>
+  </si>
+  <si>
+    <t>HR-аналитика</t>
+  </si>
+  <si>
+    <t>olymp@hse.ru</t>
+  </si>
+  <si>
+    <t>+7(852)4554545</t>
+  </si>
+  <si>
+    <t>2010-01-10</t>
+  </si>
+  <si>
+    <t>м</t>
+  </si>
+  <si>
+    <t>Магистратура 1</t>
+  </si>
+  <si>
+    <t>штаб</t>
+  </si>
+  <si>
+    <t>БэдЗапрос</t>
+  </si>
+  <si>
+    <t>2020-09-01</t>
+  </si>
+  <si>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Кулакова</t>
+  </si>
+  <si>
+    <t>Дуня</t>
+  </si>
+  <si>
+    <t>Андреевич</t>
+  </si>
+  <si>
+    <t>Юриспруденция</t>
+  </si>
+  <si>
+    <t>311@yandex.ru</t>
+  </si>
+  <si>
+    <t>8953а</t>
+  </si>
+  <si>
+    <t>2000-11-01</t>
+  </si>
+  <si>
+    <t>ж</t>
+  </si>
+  <si>
+    <t>Бакалавриат 4</t>
+  </si>
+  <si>
+    <t>Стов</t>
+  </si>
+  <si>
+    <t>Станислав</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Международные отношения</t>
+  </si>
+  <si>
+    <t>sov@edu.ru</t>
+  </si>
+  <si>
+    <t>+792209</t>
+  </si>
+  <si>
+    <t>1998-05-01</t>
+  </si>
+  <si>
+    <t>аудитория</t>
+  </si>
+  <si>
     <t>Региональный этап Всероссийской олимпиады школьников по праву</t>
   </si>
   <si>
@@ -112,15 +220,9 @@
     <t>2000-03-14</t>
   </si>
   <si>
-    <t>ж</t>
-  </si>
-  <si>
     <t>Бакалавриат 3</t>
   </si>
   <si>
-    <t>аудитория</t>
-  </si>
-  <si>
     <t>Одга</t>
   </si>
   <si>
@@ -142,12 +244,6 @@
     <t>1998-09-13</t>
   </si>
   <si>
-    <t>Бакалавриат 4</t>
-  </si>
-  <si>
-    <t>штаб</t>
-  </si>
-  <si>
     <t>Ава</t>
   </si>
   <si>
@@ -196,9 +292,6 @@
     <t xml:space="preserve">Игоревна </t>
   </si>
   <si>
-    <t>Юриспруденция</t>
-  </si>
-  <si>
     <t>lerao@mail.ru</t>
   </si>
   <si>
@@ -235,9 +328,6 @@
     <t xml:space="preserve">Маратович </t>
   </si>
   <si>
-    <t>Международные отношения</t>
-  </si>
-  <si>
     <t>yh77@gmail.com</t>
   </si>
   <si>
@@ -247,9 +337,6 @@
     <t>1997-04-13</t>
   </si>
   <si>
-    <t>м</t>
-  </si>
-  <si>
     <t>Шар</t>
   </si>
   <si>
@@ -442,9 +529,6 @@
     <t>1997-12-10</t>
   </si>
   <si>
-    <t>Магистратура 1</t>
-  </si>
-  <si>
     <t>Шер</t>
   </si>
   <si>
@@ -511,24 +595,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Стов</t>
-  </si>
-  <si>
-    <t>Станислав</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>sov@edu.ru</t>
-  </si>
-  <si>
-    <t>+792209</t>
-  </si>
-  <si>
-    <t>1998-05-01</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -562,7 +628,7 @@
     <t>1997-12-31</t>
   </si>
   <si>
-    <t>2020-07-28 00:00:00</t>
+    <t>2020-08-05 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -894,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -964,7 +1030,7 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -979,13 +1045,13 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2">
-        <v>98</v>
+        <v>542</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
@@ -1023,120 +1089,120 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F3">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H3">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F4">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H4">
-        <v>97</v>
+        <v>527</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -1144,58 +1210,58 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F5">
         <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H5">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="O5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q5" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -1203,52 +1269,52 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H6">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1262,52 +1328,52 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F7">
         <v>180</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H7">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="N7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" t="s">
         <v>68</v>
-      </c>
-      <c r="O7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>42</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1321,52 +1387,52 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>180</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H8">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="M8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="O8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="P8" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1380,58 +1446,58 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F9">
         <v>180</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H9">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="N9" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="O9" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="P9" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1439,58 +1505,58 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>180</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H10">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" t="s">
+        <v>99</v>
+      </c>
+      <c r="O10" t="s">
+        <v>100</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" t="s">
         <v>47</v>
-      </c>
-      <c r="M10" t="s">
-        <v>88</v>
-      </c>
-      <c r="N10" t="s">
-        <v>89</v>
-      </c>
-      <c r="O10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P10" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>42</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1498,58 +1564,58 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F11">
         <v>180</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H11">
-        <v>181</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="K11" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L11" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="M11" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="N11" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="O11" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="P11" t="s">
         <v>32</v>
       </c>
       <c r="Q11" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1557,58 +1623,58 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F12">
         <v>180</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H12">
-        <v>250</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="K12" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="L12" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="O12" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="P12" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="Q12" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1616,52 +1682,52 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F13">
         <v>180</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H13">
-        <v>255</v>
+        <v>107</v>
       </c>
       <c r="I13" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="J13" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="K13" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="L13" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="M13" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="N13" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="P13" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="Q13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1675,58 +1741,58 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F14">
         <v>180</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H14">
-        <v>272</v>
+        <v>181</v>
       </c>
       <c r="I14" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K14" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L14" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="M14" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="N14" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="P14" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="Q14" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1734,58 +1800,58 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F15">
         <v>180</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H15">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="J15" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="K15" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="M15" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="N15" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="O15" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="P15" t="s">
         <v>32</v>
       </c>
       <c r="Q15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1793,232 +1859,235 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F16">
         <v>180</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H16">
-        <v>295</v>
+        <v>255</v>
       </c>
       <c r="I16" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J16" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="K16" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="L16" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="M16" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="O16" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="P16" t="s">
         <v>32</v>
       </c>
       <c r="Q16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="H17">
-        <v>84</v>
+        <v>272</v>
       </c>
       <c r="I17" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="J17" t="s">
+        <v>142</v>
+      </c>
+      <c r="K17" t="s">
+        <v>143</v>
+      </c>
+      <c r="L17" t="s">
         <v>137</v>
       </c>
-      <c r="L17" t="s">
-        <v>138</v>
-      </c>
       <c r="M17" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="N17" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="O17" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="P17" t="s">
         <v>32</v>
       </c>
       <c r="Q17" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="F18">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="H18">
-        <v>460</v>
+        <v>287</v>
       </c>
       <c r="I18" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J18" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K18" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="L18" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="M18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="N18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="O18" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="P18" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q18" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="F19">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="G19" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="H19">
-        <v>500</v>
+        <v>295</v>
       </c>
       <c r="I19" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="J19" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="K19" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="M19" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="N19" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="O19" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="P19" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="Q19" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -2026,52 +2095,49 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="F20">
         <v>80</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="H20">
-        <v>442</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="J20" t="s">
-        <v>155</v>
-      </c>
-      <c r="K20" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="L20" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M20" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="N20" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="O20" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="P20" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="Q20" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -2082,10 +2148,10 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
         <v>161</v>
@@ -2097,87 +2163,84 @@
         <v>163</v>
       </c>
       <c r="F21">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
         <v>164</v>
       </c>
       <c r="H21">
-        <v>527</v>
+        <v>460</v>
       </c>
       <c r="I21" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="J21" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="K21" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="L21" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="M21" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="N21" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="O21" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="P21" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="Q21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="R21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>34</v>
-      </c>
-      <c r="T21" t="s">
-        <v>171</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="F22">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
         <v>164</v>
       </c>
       <c r="H22">
-        <v>8</v>
+        <v>500</v>
       </c>
       <c r="I22" t="s">
-        <v>175</v>
+        <v>61</v>
       </c>
       <c r="J22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L22" t="s">
-        <v>178</v>
+        <v>110</v>
       </c>
       <c r="M22" t="s">
         <v>179</v>
@@ -2189,21 +2252,201 @@
         <v>181</v>
       </c>
       <c r="P22" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>47</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23">
+        <v>442</v>
+      </c>
+      <c r="I23" t="s">
+        <v>182</v>
+      </c>
+      <c r="J23" t="s">
+        <v>183</v>
+      </c>
+      <c r="K23" t="s">
+        <v>184</v>
+      </c>
+      <c r="L23" t="s">
+        <v>185</v>
+      </c>
+      <c r="M23" t="s">
+        <v>186</v>
+      </c>
+      <c r="N23" t="s">
+        <v>187</v>
+      </c>
+      <c r="O23" t="s">
+        <v>188</v>
+      </c>
+      <c r="P23" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" t="s">
-        <v>142</v>
-      </c>
-      <c r="R22">
+      <c r="Q23" t="s">
+        <v>33</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>191</v>
+      </c>
+      <c r="F24">
+        <v>120</v>
+      </c>
+      <c r="G24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24">
+        <v>527</v>
+      </c>
+      <c r="I24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" t="s">
+        <v>53</v>
+      </c>
+      <c r="O24" t="s">
+        <v>54</v>
+      </c>
+      <c r="P24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>47</v>
+      </c>
+      <c r="R24">
         <v>1</v>
       </c>
-      <c r="S22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" t="s">
-        <v>182</v>
+      <c r="S24" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>197</v>
+      </c>
+      <c r="J25" t="s">
+        <v>198</v>
+      </c>
+      <c r="K25" t="s">
+        <v>199</v>
+      </c>
+      <c r="L25" t="s">
+        <v>200</v>
+      </c>
+      <c r="M25" t="s">
+        <v>201</v>
+      </c>
+      <c r="N25" t="s">
+        <v>202</v>
+      </c>
+      <c r="O25" t="s">
+        <v>203</v>
+      </c>
+      <c r="P25" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>33</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>